<commit_message>
add sound, display, servo, rgb led and others
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artem V\PycharmProjects\pythonProject\ПредПроф\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artem V\PycharmProjects\pythonProject\ПредПроф\RFID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27859B56-9603-40C0-B54E-2919A5DF7D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94121C7E-EAB3-4136-9854-5C6814BA08A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5445" yWindow="1500" windowWidth="21600" windowHeight="11295" xr2:uid="{24236BBD-4372-4DA4-BE3C-603A2941FBA4}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,7 +432,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>45656</v>
+        <v>45678</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new system time control and modification schemes
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artem V\PycharmProjects\pythonProject\ПредПроф\RFID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94121C7E-EAB3-4136-9854-5C6814BA08A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5245FF93-29D8-41AB-BB55-606DDBCB9C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5445" yWindow="1500" windowWidth="21600" windowHeight="11295" xr2:uid="{24236BBD-4372-4DA4-BE3C-603A2941FBA4}"/>
+    <workbookView xWindow="6645" yWindow="1980" windowWidth="21600" windowHeight="11295" xr2:uid="{24236BBD-4372-4DA4-BE3C-603A2941FBA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,7 +432,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>45678</v>
+        <v>45690</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add recognition cards one per day and rework python(a little)
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artem V\PycharmProjects\pythonProject\ПредПроф\RFID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5245FF93-29D8-41AB-BB55-606DDBCB9C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B877AA3-531A-4EAF-A442-5A7B5CFDE93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6645" yWindow="1980" windowWidth="21600" windowHeight="11295" xr2:uid="{24236BBD-4372-4DA4-BE3C-603A2941FBA4}"/>
+    <workbookView xWindow="5535" yWindow="1935" windowWidth="21600" windowHeight="11295" xr2:uid="{24236BBD-4372-4DA4-BE3C-603A2941FBA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,15 +447,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>333</v>
-      </c>
-      <c r="C4" s="1">
-        <v>45652</v>
-      </c>
+      <c r="C4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>